<commit_message>
added more tasks to todo.xlsx
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
   <si>
     <t>враговете да не се блъскат</t>
   </si>
@@ -99,10 +99,22 @@
     <t>менюта</t>
   </si>
   <si>
-    <t>ок</t>
-  </si>
-  <si>
     <t>враговете</t>
+  </si>
+  <si>
+    <t>козметични промени</t>
+  </si>
+  <si>
+    <t>GitHub</t>
+  </si>
+  <si>
+    <t>Име</t>
+  </si>
+  <si>
+    <t>TAG</t>
+  </si>
+  <si>
+    <t>задача</t>
   </si>
 </sst>
 </file>
@@ -477,10 +489,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,103 +505,102 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" t="s">
-        <v>27</v>
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" t="s">
-        <v>27</v>
+        <v>19</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>23</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>24</v>
       </c>
-      <c r="C8" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>4</v>
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>4</v>
@@ -597,31 +608,31 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>26</v>
@@ -629,9 +640,25 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B19" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added colors to tasks in todo.xlsx
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -121,7 +121,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,13 +131,19 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -146,8 +152,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -160,15 +183,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="60% - Accent1" xfId="1" builtinId="32"/>
+    <cellStyle name="60% - Accent2" xfId="3" builtinId="36"/>
+    <cellStyle name="60% - Accent3" xfId="4" builtinId="40"/>
+    <cellStyle name="Accent2" xfId="2" builtinId="33"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -492,7 +526,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,7 +563,7 @@
       <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>26</v>
       </c>
     </row>
@@ -540,7 +574,7 @@
       <c r="B4" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="4" t="s">
         <v>27</v>
       </c>
     </row>
@@ -551,7 +585,7 @@
       <c r="B5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -562,6 +596,7 @@
       <c r="B6" t="s">
         <v>22</v>
       </c>
+      <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -570,7 +605,7 @@
       <c r="B7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -599,26 +634,26 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="4" t="s">
         <v>5</v>
       </c>
     </row>
@@ -631,34 +666,34 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="3" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>